<commit_message>
Final changes for paper made
</commit_message>
<xml_diff>
--- a/CURRENT WORK/CRITICAL POINTS/Excel.xlsx
+++ b/CURRENT WORK/CRITICAL POINTS/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jda365-my.sharepoint.com/personal/dhanush_tamilselvan_jda_com/Documents/Desktop/Final-Year-Project/CURRENT WORK/CRITICAL POINTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{B8A046C5-71F8-4645-8BEA-770A99D02529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE3F027B-41E0-4312-BDBE-030634B128C1}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{B8A046C5-71F8-4645-8BEA-770A99D02529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE522477-A79E-4A17-A022-3D48F34A7E18}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{56FB4B74-5F51-4F48-B8C4-470E0A5A16D7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Volume Fraction</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Temperature Deviation</t>
-  </si>
-  <si>
-    <t>Our Work Data</t>
   </si>
   <si>
     <t>Molality Deviation</t>
@@ -143,6 +140,18 @@
       </rPr>
       <t>4</t>
     </r>
+  </si>
+  <si>
+    <t>Our Model eq 16 &amp; 17</t>
+  </si>
+  <si>
+    <t>Critical Temperature</t>
+  </si>
+  <si>
+    <t>Critical Molality</t>
+  </si>
+  <si>
+    <t>Salts</t>
   </si>
 </sst>
 </file>
@@ -273,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,9 +314,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -326,6 +332,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -648,7 +658,7 @@
   <dimension ref="C3:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H12" sqref="H12:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -703,8 +713,8 @@
       <c r="L5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="15" t="s">
-        <v>13</v>
+      <c r="M5" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.35">
@@ -874,7 +884,7 @@
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.35">
       <c r="I12" s="14" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" t="s">
@@ -882,26 +892,29 @@
       </c>
     </row>
     <row r="13" spans="3:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I13" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="16" t="s">
+      <c r="N13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.35">
@@ -910,7 +923,7 @@
         <v>-10.932201008676131</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I14" s="1">
         <v>3.9363513764215585</v>
@@ -928,15 +941,15 @@
         <v>2.7298657266636122</v>
       </c>
       <c r="N14">
-        <v>2.1575868845358581</v>
+        <v>-10.932201008676131</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.35">
       <c r="H15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15" s="1">
         <v>3.4503826903753825</v>
@@ -957,7 +970,7 @@
         <v>1.9499093385796431</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.35">
@@ -983,7 +996,7 @@
         <v>5.6648763259418278</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="8:15" x14ac:dyDescent="0.35">
@@ -1009,7 +1022,7 @@
         <v>5.2345595138193826</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="8:15" x14ac:dyDescent="0.35">
@@ -1035,7 +1048,7 @@
         <v>4.4625555400732226</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>